<commit_message>
Add edit functionality for Excel data AI recommendations in output page: implement edit button, reason input, and validation similar to input page
</commit_message>
<xml_diff>
--- a/frontend/public/templates/실적_데이터_아웃풋.xlsx
+++ b/frontend/public/templates/실적_데이터_아웃풋.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sdhg\Documents\카카오톡 받은 파일\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sdhg\Desktop\greensteel-main\frontend\public\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CFEBE43-2953-43DD-8661-EFBCF811BA52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E25CCC9D-31A3-4569-B607-6EBFB97F65D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23385" yWindow="7260" windowWidth="23385" windowHeight="7140" xr2:uid="{82767D5A-7309-4993-B26A-A005DB64C41C}"/>
+    <workbookView xWindow="1035" yWindow="3645" windowWidth="25725" windowHeight="8415" xr2:uid="{82767D5A-7309-4993-B26A-A005DB64C41C}"/>
   </bookViews>
   <sheets>
     <sheet name="그리드(실적정보)" sheetId="1" r:id="rId1"/>
@@ -783,7 +783,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="45">
   <si>
     <t>수량</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -825,14 +825,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>OO건설</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ㅁㅁ철강</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>XX 자동차</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -842,6 +834,133 @@
   </si>
   <si>
     <t>산출물_단위</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>삼정 자동차</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>블룸</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>코크스 생산</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>점결탄</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>T</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>소결</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>광석</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>정립광</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>석회</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>코크스 오븐 코크스</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>제선</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>철ㄹ</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Coke</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>제강</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>열유입</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>KJ</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>주조</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>KP 철강</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>냉각수</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ㅎ놘철</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>빌렛</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>환ㅇ웣널</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MG건설</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EAF 탄소 전극</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>물</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>L</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>형강</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>압연</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>요소수</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>포장</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>포장재</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -902,7 +1021,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -912,6 +1031,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -945,7 +1082,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -958,7 +1095,25 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="6" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1277,8 +1432,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4C89ADB-7F75-4E54-9CD4-F11D122E1D13}">
   <dimension ref="A1:L22"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:L20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1309,7 +1464,7 @@
         <v>5</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>4</v>
@@ -1327,354 +1482,734 @@
         <v>0</v>
       </c>
       <c r="L1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="33" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="4">
+        <v>716926</v>
+      </c>
+      <c r="C2" s="4">
+        <v>1</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>14</v>
       </c>
+      <c r="E2" s="4">
+        <v>20</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="6">
+        <v>45870</v>
+      </c>
+      <c r="H2" s="6">
+        <v>45873</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="K2" s="4">
+        <v>1</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" s="1">
+    <row r="3" spans="1:12" ht="33" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="4">
         <v>716926</v>
       </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="1"/>
+      <c r="C3" s="4">
+        <v>1</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="4">
+        <v>20</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" s="6">
+        <v>45871</v>
+      </c>
+      <c r="H3" s="6">
+        <v>45872</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="K3" s="4">
+        <v>1</v>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="1">
+    <row r="4" spans="1:12" ht="33" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="4">
         <v>716926</v>
       </c>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
-      <c r="L3" s="1"/>
+      <c r="C4" s="4">
+        <v>1</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="4">
+        <v>20</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" s="6">
+        <v>45871</v>
+      </c>
+      <c r="H4" s="6">
+        <v>45872</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="K4" s="4">
+        <v>3</v>
+      </c>
+      <c r="L4" s="4" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="1">
+    <row r="5" spans="1:12" ht="33" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="4">
         <v>716926</v>
       </c>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
-      <c r="L4" s="1"/>
+      <c r="C5" s="4">
+        <v>1</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="4">
+        <v>20</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5" s="6">
+        <v>45872</v>
+      </c>
+      <c r="H5" s="6">
+        <v>45873</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J5" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="K5" s="4">
+        <v>2</v>
+      </c>
+      <c r="L5" s="4" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="1">
+    <row r="6" spans="1:12" ht="33" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="4">
         <v>716926</v>
       </c>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
-      <c r="L5" s="1"/>
+      <c r="C6" s="4">
+        <v>1</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" s="4">
+        <v>20</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G6" s="6">
+        <v>45872</v>
+      </c>
+      <c r="H6" s="6">
+        <v>45873</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J6" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="K6" s="4">
+        <v>2</v>
+      </c>
+      <c r="L6" s="4" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="1">
+    <row r="7" spans="1:12" ht="33" x14ac:dyDescent="0.3">
+      <c r="A7" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="4">
         <v>716926</v>
       </c>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3"/>
-      <c r="L6" s="1"/>
+      <c r="C7" s="4">
+        <v>1</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" s="4">
+        <v>20</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G7" s="6">
+        <v>45873</v>
+      </c>
+      <c r="H7" s="6">
+        <v>45875</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="J7" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="K7" s="4">
+        <v>5</v>
+      </c>
+      <c r="L7" s="4" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="1">
+    <row r="8" spans="1:12" ht="33" x14ac:dyDescent="0.3">
+      <c r="A8" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="4">
         <v>716926</v>
       </c>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
-      <c r="K7" s="3"/>
-      <c r="L7" s="1"/>
+      <c r="C8" s="4">
+        <v>1</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" s="4">
+        <v>20</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G8" s="6">
+        <v>45873</v>
+      </c>
+      <c r="H8" s="6">
+        <v>45875</v>
+      </c>
+      <c r="I8" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="J8" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="K8" s="4">
+        <v>5</v>
+      </c>
+      <c r="L8" s="4" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" s="1">
+    <row r="9" spans="1:12" ht="33" x14ac:dyDescent="0.3">
+      <c r="A9" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="4">
         <v>716926</v>
       </c>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
-      <c r="K8" s="3"/>
-      <c r="L8" s="1"/>
+      <c r="C9" s="4">
+        <v>1</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" s="4">
+        <v>20</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G9" s="6">
+        <v>45873</v>
+      </c>
+      <c r="H9" s="6">
+        <v>45875</v>
+      </c>
+      <c r="I9" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="J9" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="K9" s="4">
+        <v>1</v>
+      </c>
+      <c r="L9" s="4" t="s">
+        <v>29</v>
+      </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" s="1">
+    <row r="10" spans="1:12" ht="33" x14ac:dyDescent="0.3">
+      <c r="A10" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="4">
         <v>716926</v>
       </c>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="3"/>
-      <c r="J9" s="3"/>
-      <c r="K9" s="3"/>
-      <c r="L9" s="1"/>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10" s="1">
-        <v>716926</v>
-      </c>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
-      <c r="I10" s="3"/>
-      <c r="J10" s="3"/>
-      <c r="K10" s="3"/>
-      <c r="L10" s="1"/>
+      <c r="C10" s="4">
+        <v>1</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="E10" s="4">
+        <v>20</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G10" s="6">
+        <v>45875</v>
+      </c>
+      <c r="H10" s="6">
+        <v>45878</v>
+      </c>
+      <c r="I10" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="J10" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="K10" s="4">
+        <v>4</v>
+      </c>
+      <c r="L10" s="4" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11" s="1">
-        <v>716926</v>
-      </c>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4"/>
-      <c r="I11" s="3"/>
-      <c r="J11" s="3"/>
-      <c r="K11" s="3"/>
-      <c r="L11" s="1"/>
+      <c r="A11" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" s="4">
+        <v>771260</v>
+      </c>
+      <c r="C11" s="4">
+        <v>2</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E11" s="4">
+        <v>20</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G11" s="6">
+        <v>45872</v>
+      </c>
+      <c r="H11" s="6">
+        <v>45875</v>
+      </c>
+      <c r="I11" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="J11" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="K11" s="4">
+        <v>3</v>
+      </c>
+      <c r="L11" s="4" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B12" s="1">
-        <v>716926</v>
-      </c>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="4"/>
-      <c r="I12" s="3"/>
-      <c r="J12" s="3"/>
-      <c r="K12" s="3"/>
-      <c r="L12" s="1"/>
+      <c r="A12" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" s="4">
+        <v>771260</v>
+      </c>
+      <c r="C12" s="4">
+        <v>2</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E12" s="4">
+        <v>20</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G12" s="6">
+        <v>45877</v>
+      </c>
+      <c r="H12" s="6">
+        <v>45880</v>
+      </c>
+      <c r="I12" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="J12" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="K12" s="4">
+        <v>2</v>
+      </c>
+      <c r="L12" s="4" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A13" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B13" s="1">
-        <v>716926</v>
-      </c>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="2"/>
-      <c r="I13" s="3"/>
-      <c r="J13" s="3"/>
-      <c r="K13" s="3"/>
-      <c r="L13" s="1"/>
+      <c r="A13" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" s="4">
+        <v>771260</v>
+      </c>
+      <c r="C13" s="4">
+        <v>2</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E13" s="4">
+        <v>20</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G13" s="6">
+        <v>45877</v>
+      </c>
+      <c r="H13" s="6">
+        <v>45880</v>
+      </c>
+      <c r="I13" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="J13" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="K13" s="4">
+        <v>3</v>
+      </c>
+      <c r="L13" s="4" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A14" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B14" s="1">
-        <v>716926</v>
-      </c>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="2"/>
-      <c r="I14" s="3"/>
-      <c r="J14" s="3"/>
-      <c r="K14" s="3"/>
-      <c r="L14" s="1"/>
+      <c r="A14" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B14" s="4">
+        <v>9265907</v>
+      </c>
+      <c r="C14" s="4">
+        <v>3</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E14" s="4">
+        <v>20</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G14" s="6">
+        <v>45881</v>
+      </c>
+      <c r="H14" s="6">
+        <v>45884</v>
+      </c>
+      <c r="I14" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="J14" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="K14" s="4">
+        <v>2</v>
+      </c>
+      <c r="L14" s="4" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A15" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B15" s="1">
-        <v>771260</v>
-      </c>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
-      <c r="I15" s="3"/>
-      <c r="J15" s="3"/>
-      <c r="K15" s="3"/>
-      <c r="L15" s="1"/>
+      <c r="A15" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B15" s="4">
+        <v>9265907</v>
+      </c>
+      <c r="C15" s="4">
+        <v>3</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E15" s="4">
+        <v>20</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G15" s="6">
+        <v>45884</v>
+      </c>
+      <c r="H15" s="6">
+        <v>45887</v>
+      </c>
+      <c r="I15" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="J15" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="K15" s="4">
+        <v>5</v>
+      </c>
+      <c r="L15" s="4" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A16" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B16" s="1">
-        <v>771260</v>
-      </c>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="2"/>
-      <c r="H16" s="2"/>
-      <c r="I16" s="3"/>
-      <c r="J16" s="3"/>
-      <c r="K16" s="3"/>
-      <c r="L16" s="1"/>
+      <c r="A16" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B16" s="4">
+        <v>9265907</v>
+      </c>
+      <c r="C16" s="4">
+        <v>4</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="E16" s="4">
+        <v>20</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G16" s="6">
+        <v>45884</v>
+      </c>
+      <c r="H16" s="6">
+        <v>45887</v>
+      </c>
+      <c r="I16" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="J16" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="K16" s="4">
+        <v>5</v>
+      </c>
+      <c r="L16" s="4" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A17" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B17" s="1">
-        <v>771260</v>
-      </c>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-      <c r="G17" s="2"/>
-      <c r="H17" s="2"/>
-      <c r="I17" s="3"/>
-      <c r="J17" s="3"/>
-      <c r="K17" s="3"/>
-      <c r="L17" s="1"/>
+      <c r="A17" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B17" s="4">
+        <v>9265907</v>
+      </c>
+      <c r="C17" s="4">
+        <v>4</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="E17" s="4">
+        <v>20</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G17" s="6">
+        <v>45884</v>
+      </c>
+      <c r="H17" s="6">
+        <v>45887</v>
+      </c>
+      <c r="I17" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="J17" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="K17" s="4">
+        <v>5</v>
+      </c>
+      <c r="L17" s="4" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A18" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B18" s="1">
-        <v>771260</v>
-      </c>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
-      <c r="G18" s="2"/>
-      <c r="H18" s="2"/>
-      <c r="I18" s="3"/>
-      <c r="J18" s="3"/>
-      <c r="K18" s="3"/>
-      <c r="L18" s="1"/>
+      <c r="A18" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B18" s="4">
+        <v>9265907</v>
+      </c>
+      <c r="C18" s="4">
+        <v>4</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="E18" s="4">
+        <v>20</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G18" s="6">
+        <v>45884</v>
+      </c>
+      <c r="H18" s="6">
+        <v>45887</v>
+      </c>
+      <c r="I18" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="J18" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="K18" s="4">
+        <v>5</v>
+      </c>
+      <c r="L18" s="4" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A19" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B19" s="1">
-        <v>771260</v>
-      </c>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
-      <c r="G19" s="2"/>
-      <c r="H19" s="2"/>
-      <c r="I19" s="3"/>
-      <c r="J19" s="3"/>
-      <c r="K19" s="3"/>
-      <c r="L19" s="1"/>
+      <c r="A19" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19" s="4">
+        <v>9265907</v>
+      </c>
+      <c r="C19" s="4">
+        <v>4</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="E19" s="4">
+        <v>20</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G19" s="6">
+        <v>45884</v>
+      </c>
+      <c r="H19" s="6">
+        <v>45887</v>
+      </c>
+      <c r="I19" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="J19" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="K19" s="4">
+        <v>5</v>
+      </c>
+      <c r="L19" s="4" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A20" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B20" s="1">
+      <c r="A20" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B20" s="4">
         <v>9265907</v>
       </c>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
-      <c r="G20" s="2"/>
-      <c r="H20" s="2"/>
-      <c r="I20" s="3"/>
-      <c r="J20" s="3"/>
-      <c r="K20" s="3"/>
-      <c r="L20" s="1"/>
+      <c r="C20" s="4">
+        <v>4</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="E20" s="4">
+        <v>20</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G20" s="6">
+        <v>45884</v>
+      </c>
+      <c r="H20" s="6">
+        <v>45887</v>
+      </c>
+      <c r="I20" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="J20" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="K20" s="4">
+        <v>5</v>
+      </c>
+      <c r="L20" s="4" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B21" s="1">
         <v>9265907</v>
@@ -1692,7 +2227,7 @@
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B22" s="1">
         <v>9265907</v>

</xml_diff>